<commit_message>
Added support for URL's
</commit_message>
<xml_diff>
--- a/test/data/Onderwijs_changes.xlsx
+++ b/test/data/Onderwijs_changes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arjen/Library/CloudStorage/Dropbox/Development/crunch_uml/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB7B7E3-B0C8-6147-AF83-A2ED554A6427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BF3D8A-DA9C-2A49-996B-452E60133344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="760" windowWidth="26700" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>id</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>definitie</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>noval</t>
   </si>
 </sst>
 </file>
@@ -537,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -549,9 +555,10 @@
     <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,8 +580,11 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -587,8 +597,11 @@
       <c r="E2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -601,8 +614,11 @@
       <c r="E3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -615,8 +631,11 @@
       <c r="E4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -629,8 +648,11 @@
       <c r="E5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -643,8 +665,11 @@
       <c r="E6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -657,8 +682,11 @@
       <c r="E7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -674,8 +702,11 @@
       <c r="E8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -688,8 +719,11 @@
       <c r="E9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -702,8 +736,11 @@
       <c r="G10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -716,8 +753,11 @@
       <c r="E11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -733,8 +773,11 @@
       <c r="E12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -747,8 +790,11 @@
       <c r="E13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -761,8 +807,11 @@
       <c r="G14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -775,8 +824,11 @@
       <c r="E15" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -789,8 +841,11 @@
       <c r="E16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -799,6 +854,9 @@
       </c>
       <c r="E17" t="s">
         <v>46</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>